<commit_message>
rapport séance 1 krausener
</commit_message>
<xml_diff>
--- a/documentation/PLANNING.xlsx
+++ b/documentation/PLANNING.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexandre\Desktop\Alex\Cimino-Krausener-PEIP2-ARDUINO-PROJECT-\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CF6131C-F736-4B1F-9367-5DA3754E0CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FEDB95C-6E85-4445-99BC-A40C6863F313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="2500" windowWidth="14400" windowHeight="7360" xr2:uid="{93472EC9-AD6A-41AA-9B02-F118DFDDF243}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{93472EC9-AD6A-41AA-9B02-F118DFDDF243}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>PROJET ARDUINO</t>
   </si>
@@ -63,40 +64,37 @@
     <t>CIMINO</t>
   </si>
   <si>
-    <t>code déplacements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fin du code déplacement </t>
-  </si>
-  <si>
-    <t>fin du code relation voiture/déplacement</t>
-  </si>
-  <si>
-    <t>imprimer les pièces 3D/ commencer le code concernant les deplacements</t>
-  </si>
-  <si>
-    <t>code concernant la relation voiture/télécomande</t>
-  </si>
-  <si>
     <t>assemblage voiture</t>
   </si>
   <si>
-    <t>commande batteries, moteur... / commencer le code concernant la relation voiture/télécomande</t>
-  </si>
-  <si>
-    <t>gestion marche arrière</t>
-  </si>
-  <si>
-    <t>code déplacements + assemblage voiture</t>
-  </si>
-  <si>
-    <t>code concernant la relation voiture/télécomande + assemblage voiture</t>
-  </si>
-  <si>
     <t>pimpage de la caisse</t>
   </si>
   <si>
     <t xml:space="preserve">pimpage de la caisse </t>
+  </si>
+  <si>
+    <t>recherche information moteur/ achat pièce moteur/batterie</t>
+  </si>
+  <si>
+    <t>recherche informations transmission, cerveau moteur, achat pièces complemetaires</t>
+  </si>
+  <si>
+    <t>développement pièces transmission</t>
+  </si>
+  <si>
+    <t>développement pièces direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imprimer pièces faites au td d'avant </t>
+  </si>
+  <si>
+    <t>gestion direction avec télécomande (code)</t>
+  </si>
+  <si>
+    <t>gestion vitesse avec télécommande</t>
+  </si>
+  <si>
+    <t>création télécommande</t>
   </si>
 </sst>
 </file>
@@ -461,7 +459,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -498,7 +496,7 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -509,10 +507,10 @@
         <v>45282</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -523,10 +521,10 @@
         <v>45303</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -537,10 +535,10 @@
         <v>45310</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -551,10 +549,10 @@
         <v>45316</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -564,8 +562,11 @@
       <c r="B8" s="1">
         <v>45330</v>
       </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -575,6 +576,12 @@
       <c r="B9" s="1">
         <v>45337</v>
       </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -584,10 +591,10 @@
         <v>45344</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>